<commit_message>
new data scraped and working on odds module finishing touches :)
</commit_message>
<xml_diff>
--- a/Odds/NCAAF/ncaa football 2020-21.xlsx
+++ b/Odds/NCAAF/ncaa football 2020-21.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nate\Documents\My Web Sites\Sportsbook Reviews Online\scoresoddsarchives\ncaafootball\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DFE20FC6-5360-4606-AD17-EF6C66271C69}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4ABDCC2-A434-4780-9EF5-A58125FA84F1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17790" xr2:uid="{7C07D7E8-10EF-4D13-AFBA-D329EF6643CB}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="741" uniqueCount="111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="935" uniqueCount="136">
   <si>
     <t>Date</t>
   </si>
@@ -366,6 +366,81 @@
   </si>
   <si>
     <t>Massachusetts</t>
+  </si>
+  <si>
+    <t>Illinois</t>
+  </si>
+  <si>
+    <t>Wisconsin</t>
+  </si>
+  <si>
+    <t>PennState</t>
+  </si>
+  <si>
+    <t>Indiana</t>
+  </si>
+  <si>
+    <t>Rutgers</t>
+  </si>
+  <si>
+    <t>MichiganState</t>
+  </si>
+  <si>
+    <t>Nebraska</t>
+  </si>
+  <si>
+    <t>OhioState</t>
+  </si>
+  <si>
+    <t>Iowa</t>
+  </si>
+  <si>
+    <t>Purdue</t>
+  </si>
+  <si>
+    <t>Maryland</t>
+  </si>
+  <si>
+    <t>Northwestern</t>
+  </si>
+  <si>
+    <t>UtahState</t>
+  </si>
+  <si>
+    <t>BoiseState</t>
+  </si>
+  <si>
+    <t>Hawaii</t>
+  </si>
+  <si>
+    <t>FresnoState</t>
+  </si>
+  <si>
+    <t>UNLV</t>
+  </si>
+  <si>
+    <t>SanDiegoState</t>
+  </si>
+  <si>
+    <t>SanJoseState</t>
+  </si>
+  <si>
+    <t>Wyoming</t>
+  </si>
+  <si>
+    <t>Nevada</t>
+  </si>
+  <si>
+    <t>Michigan</t>
+  </si>
+  <si>
+    <t>Minnesota</t>
+  </si>
+  <si>
+    <t>Rice</t>
+  </si>
+  <si>
+    <t>Chattanooga</t>
   </si>
 </sst>
 </file>
@@ -7756,7 +7831,7 @@
         <v>-1600</v>
       </c>
       <c r="M171" s="2">
-        <v>-10</v>
+        <v>10</v>
       </c>
     </row>
     <row r="172" spans="1:13" x14ac:dyDescent="0.15">
@@ -7838,7 +7913,7 @@
         <v>-700</v>
       </c>
       <c r="M173" s="2">
-        <v>-7</v>
+        <v>7</v>
       </c>
     </row>
     <row r="174" spans="1:13" x14ac:dyDescent="0.15">
@@ -7879,7 +7954,7 @@
         <v>-125</v>
       </c>
       <c r="M174" s="2">
-        <v>-2.5</v>
+        <v>2.5</v>
       </c>
     </row>
     <row r="175" spans="1:13" x14ac:dyDescent="0.15">
@@ -7961,7 +8036,7 @@
         <v>-600</v>
       </c>
       <c r="M176" s="2">
-        <v>-7</v>
+        <v>7</v>
       </c>
     </row>
     <row r="177" spans="1:13" x14ac:dyDescent="0.15">
@@ -8043,7 +8118,7 @@
         <v>-400</v>
       </c>
       <c r="M178" s="2">
-        <v>-5</v>
+        <v>5</v>
       </c>
     </row>
     <row r="179" spans="1:13" x14ac:dyDescent="0.15">
@@ -8247,8 +8322,8 @@
       <c r="L183" s="2">
         <v>105</v>
       </c>
-      <c r="M183" s="2" t="s">
-        <v>92</v>
+      <c r="M183" s="2">
+        <v>24.5</v>
       </c>
     </row>
     <row r="184" spans="1:13" x14ac:dyDescent="0.15">
@@ -8330,7 +8405,7 @@
         <v>-5000</v>
       </c>
       <c r="M185" s="2">
-        <v>-10.5</v>
+        <v>10.5</v>
       </c>
     </row>
     <row r="186" spans="1:13" x14ac:dyDescent="0.15">
@@ -8412,7 +8487,7 @@
         <v>-600</v>
       </c>
       <c r="M187" s="2">
-        <v>-7</v>
+        <v>7</v>
       </c>
     </row>
     <row r="188" spans="1:13" x14ac:dyDescent="0.15">
@@ -8453,7 +8528,7 @@
         <v>-290</v>
       </c>
       <c r="M188" s="2">
-        <v>-2.5</v>
+        <v>2.5</v>
       </c>
     </row>
     <row r="189" spans="1:13" x14ac:dyDescent="0.15">
@@ -8535,7 +8610,7 @@
         <v>105</v>
       </c>
       <c r="M190" s="2">
-        <v>-1</v>
+        <v>1</v>
       </c>
     </row>
     <row r="191" spans="1:13" x14ac:dyDescent="0.15">
@@ -8658,7 +8733,7 @@
         <v>-1200</v>
       </c>
       <c r="M193" s="2">
-        <v>-8</v>
+        <v>8</v>
       </c>
     </row>
     <row r="194" spans="1:13" x14ac:dyDescent="0.15">
@@ -8699,7 +8774,7 @@
         <v>-170</v>
       </c>
       <c r="M194" s="2">
-        <v>-3</v>
+        <v>3</v>
       </c>
     </row>
     <row r="195" spans="1:13" x14ac:dyDescent="0.15">
@@ -8863,7 +8938,7 @@
         <v>-110</v>
       </c>
       <c r="M198" s="2">
-        <v>-3</v>
+        <v>3</v>
       </c>
     </row>
     <row r="199" spans="1:13" x14ac:dyDescent="0.15">
@@ -8945,7 +9020,7 @@
         <v>-1800</v>
       </c>
       <c r="M200" s="2">
-        <v>-10</v>
+        <v>10</v>
       </c>
     </row>
     <row r="201" spans="1:13" x14ac:dyDescent="0.15">
@@ -9068,7 +9143,7 @@
         <v>-2000</v>
       </c>
       <c r="M203" s="2">
-        <v>-10.5</v>
+        <v>10.5</v>
       </c>
     </row>
     <row r="204" spans="1:13" x14ac:dyDescent="0.15">
@@ -9150,7 +9225,7 @@
         <v>-400</v>
       </c>
       <c r="M205" s="2">
-        <v>-5</v>
+        <v>5</v>
       </c>
     </row>
     <row r="206" spans="1:13" x14ac:dyDescent="0.15">
@@ -9232,7 +9307,7 @@
         <v>-1100</v>
       </c>
       <c r="M207" s="2">
-        <v>-7</v>
+        <v>7</v>
       </c>
     </row>
     <row r="208" spans="1:13" x14ac:dyDescent="0.15">
@@ -9314,7 +9389,7 @@
         <v>-260</v>
       </c>
       <c r="M209" s="2">
-        <v>-3</v>
+        <v>3</v>
       </c>
     </row>
     <row r="210" spans="1:13" x14ac:dyDescent="0.15">
@@ -9355,7 +9430,7 @@
         <v>-265</v>
       </c>
       <c r="M210" s="2">
-        <v>-3.5</v>
+        <v>3.5</v>
       </c>
     </row>
     <row r="211" spans="1:13" x14ac:dyDescent="0.15">
@@ -9478,7 +9553,7 @@
         <v>-200</v>
       </c>
       <c r="M213" s="2">
-        <v>-2</v>
+        <v>2</v>
       </c>
     </row>
     <row r="214" spans="1:13" x14ac:dyDescent="0.15">
@@ -9519,7 +9594,7 @@
         <v>-1400</v>
       </c>
       <c r="M214" s="2">
-        <v>-9.5</v>
+        <v>9.5</v>
       </c>
     </row>
     <row r="215" spans="1:13" x14ac:dyDescent="0.15">
@@ -9642,7 +9717,7 @@
         <v>-280</v>
       </c>
       <c r="M217" s="2">
-        <v>-2.5</v>
+        <v>2.5</v>
       </c>
     </row>
     <row r="218" spans="1:13" x14ac:dyDescent="0.15">
@@ -9683,7 +9758,7 @@
         <v>-1600</v>
       </c>
       <c r="M218" s="2">
-        <v>-9.5</v>
+        <v>9.5</v>
       </c>
     </row>
     <row r="219" spans="1:13" x14ac:dyDescent="0.15">
@@ -9806,7 +9881,7 @@
         <v>-900</v>
       </c>
       <c r="M221" s="2">
-        <v>-9</v>
+        <v>9</v>
       </c>
     </row>
     <row r="222" spans="1:13" x14ac:dyDescent="0.15">
@@ -9888,7 +9963,7 @@
         <v>-125</v>
       </c>
       <c r="M223" s="2">
-        <v>-2</v>
+        <v>2</v>
       </c>
     </row>
     <row r="224" spans="1:13" x14ac:dyDescent="0.15">
@@ -9970,7 +10045,7 @@
         <v>80</v>
       </c>
       <c r="M225" s="2">
-        <v>-14.5</v>
+        <v>14.5</v>
       </c>
     </row>
     <row r="226" spans="1:13" x14ac:dyDescent="0.15">
@@ -10052,7 +10127,7 @@
         <v>80</v>
       </c>
       <c r="M227" s="2">
-        <v>-11</v>
+        <v>11</v>
       </c>
     </row>
     <row r="228" spans="1:13" x14ac:dyDescent="0.15">
@@ -10134,7 +10209,7 @@
         <v>-4000</v>
       </c>
       <c r="M229" s="2">
-        <v>-14.5</v>
+        <v>14.5</v>
       </c>
     </row>
     <row r="230" spans="1:13" x14ac:dyDescent="0.15">
@@ -15226,109 +15301,3956 @@
       <c r="N353" s="3"/>
     </row>
     <row r="354" spans="1:14" x14ac:dyDescent="0.15">
-      <c r="M354" s="3"/>
-      <c r="N354" s="3"/>
+      <c r="A354" s="2">
+        <v>1022</v>
+      </c>
+      <c r="B354" s="2">
+        <v>305</v>
+      </c>
+      <c r="C354" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D354" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="E354" s="2">
+        <v>7</v>
+      </c>
+      <c r="F354" s="2">
+        <v>0</v>
+      </c>
+      <c r="G354" s="2">
+        <v>10</v>
+      </c>
+      <c r="H354" s="2">
+        <v>0</v>
+      </c>
+      <c r="I354" s="2">
+        <v>17</v>
+      </c>
+      <c r="J354" s="2">
+        <v>63</v>
+      </c>
+      <c r="K354" s="2">
+        <v>69.5</v>
+      </c>
+      <c r="L354" s="2">
+        <v>425</v>
+      </c>
+      <c r="M354" s="2">
+        <v>31</v>
+      </c>
     </row>
     <row r="355" spans="1:14" x14ac:dyDescent="0.15">
-      <c r="M355" s="3"/>
-      <c r="N355" s="3"/>
-    </row>
-    <row r="369" ht="9" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="370" ht="9" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="371" ht="9" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="372" ht="9" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="373" ht="9" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="374" ht="9" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="375" ht="9" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="376" ht="9" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="377" ht="9" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="378" ht="9" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="379" ht="9" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="380" ht="9" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="381" ht="9" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="382" ht="9" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="383" ht="9" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="384" ht="9" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="385" ht="9" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="386" ht="9" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="387" ht="9" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="388" ht="9" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="389" ht="9" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="390" ht="9" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="391" ht="9" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="392" ht="9" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="393" ht="9" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="394" ht="9" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="395" ht="9" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="396" ht="9" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="397" ht="9" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="398" ht="9" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="399" ht="9" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="400" ht="9" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="401" ht="9" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="402" ht="9" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="403" ht="9" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="404" ht="9" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="405" ht="9" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="406" ht="9" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="407" ht="9" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="408" ht="9" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="409" ht="9" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="410" ht="9" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="411" ht="9" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="412" ht="9" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="413" ht="9" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="414" ht="9" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="415" ht="9" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="416" ht="9" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="417" ht="9" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="418" ht="9" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="419" ht="9" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="420" ht="9" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="421" ht="9" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="422" ht="9" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="423" ht="9" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="424" ht="9" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="425" ht="9" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="426" ht="9" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="427" ht="9" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="428" ht="9" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="429" ht="9" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="430" ht="9" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="431" ht="9" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="432" ht="9" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="433" ht="9" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="434" ht="9" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="435" ht="9" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="436" ht="9" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="437" ht="9" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="438" ht="9" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="439" ht="9" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="440" ht="9" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="441" ht="9" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="442" ht="9" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="443" ht="9" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="444" ht="9" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="445" ht="9" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="446" ht="9" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="447" ht="9" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="448" ht="9" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="449" ht="9" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="450" ht="9" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="451" ht="9" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="452" ht="9" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="453" ht="9" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="454" ht="9" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="455" ht="9" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="456" ht="9" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="457" ht="9" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="458" ht="9" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="459" ht="9" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="460" ht="9" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="461" ht="9" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="462" ht="9" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="463" ht="9" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="464" ht="9" customHeight="1" x14ac:dyDescent="0.15"/>
+      <c r="A355" s="2">
+        <v>1022</v>
+      </c>
+      <c r="B355" s="2">
+        <v>306</v>
+      </c>
+      <c r="C355" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D355" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="E355" s="2">
+        <v>14</v>
+      </c>
+      <c r="F355" s="2">
+        <v>17</v>
+      </c>
+      <c r="G355" s="2">
+        <v>7</v>
+      </c>
+      <c r="H355" s="2">
+        <v>7</v>
+      </c>
+      <c r="I355" s="2">
+        <v>45</v>
+      </c>
+      <c r="J355" s="2">
+        <v>10.5</v>
+      </c>
+      <c r="K355" s="2">
+        <v>14</v>
+      </c>
+      <c r="L355" s="2">
+        <v>-550</v>
+      </c>
+      <c r="M355" s="2">
+        <v>6.5</v>
+      </c>
+    </row>
+    <row r="356" spans="1:14" x14ac:dyDescent="0.15">
+      <c r="A356" s="2">
+        <v>1023</v>
+      </c>
+      <c r="B356" s="2">
+        <v>307</v>
+      </c>
+      <c r="C356" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D356" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="E356" s="2">
+        <v>7</v>
+      </c>
+      <c r="F356" s="2">
+        <v>14</v>
+      </c>
+      <c r="G356" s="2">
+        <v>21</v>
+      </c>
+      <c r="H356" s="2">
+        <v>0</v>
+      </c>
+      <c r="I356" s="2">
+        <v>42</v>
+      </c>
+      <c r="J356" s="2">
+        <v>10</v>
+      </c>
+      <c r="K356" s="2">
+        <v>12</v>
+      </c>
+      <c r="L356" s="2">
+        <v>-450</v>
+      </c>
+      <c r="M356" s="2">
+        <v>6.5</v>
+      </c>
+    </row>
+    <row r="357" spans="1:14" x14ac:dyDescent="0.15">
+      <c r="A357" s="2">
+        <v>1023</v>
+      </c>
+      <c r="B357" s="2">
+        <v>308</v>
+      </c>
+      <c r="C357" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D357" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="E357" s="2">
+        <v>6</v>
+      </c>
+      <c r="F357" s="2">
+        <v>0</v>
+      </c>
+      <c r="G357" s="2">
+        <v>7</v>
+      </c>
+      <c r="H357" s="2">
+        <v>0</v>
+      </c>
+      <c r="I357" s="2">
+        <v>13</v>
+      </c>
+      <c r="J357" s="2">
+        <v>51</v>
+      </c>
+      <c r="K357" s="2">
+        <v>50.5</v>
+      </c>
+      <c r="L357" s="2">
+        <v>375</v>
+      </c>
+      <c r="M357" s="2">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="358" spans="1:14" x14ac:dyDescent="0.15">
+      <c r="A358" s="2">
+        <v>1023</v>
+      </c>
+      <c r="B358" s="2">
+        <v>309</v>
+      </c>
+      <c r="C358" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D358" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="E358" s="2">
+        <v>0</v>
+      </c>
+      <c r="F358" s="2">
+        <v>10</v>
+      </c>
+      <c r="G358" s="2">
+        <v>7</v>
+      </c>
+      <c r="H358" s="2">
+        <v>7</v>
+      </c>
+      <c r="I358" s="2">
+        <v>24</v>
+      </c>
+      <c r="J358" s="2">
+        <v>2</v>
+      </c>
+      <c r="K358" s="2">
+        <v>2.5</v>
+      </c>
+      <c r="L358" s="2">
+        <v>-140</v>
+      </c>
+      <c r="M358" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="359" spans="1:14" x14ac:dyDescent="0.15">
+      <c r="A359" s="2">
+        <v>1023</v>
+      </c>
+      <c r="B359" s="2">
+        <v>310</v>
+      </c>
+      <c r="C359" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D359" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="E359" s="2">
+        <v>3</v>
+      </c>
+      <c r="F359" s="2">
+        <v>10</v>
+      </c>
+      <c r="G359" s="2">
+        <v>7</v>
+      </c>
+      <c r="H359" s="2">
+        <v>0</v>
+      </c>
+      <c r="I359" s="2">
+        <v>20</v>
+      </c>
+      <c r="J359" s="2">
+        <v>49</v>
+      </c>
+      <c r="K359" s="2">
+        <v>50.5</v>
+      </c>
+      <c r="L359" s="2">
+        <v>120</v>
+      </c>
+      <c r="M359" s="2">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="360" spans="1:14" x14ac:dyDescent="0.15">
+      <c r="A360" s="2">
+        <v>1023</v>
+      </c>
+      <c r="B360" s="2">
+        <v>387</v>
+      </c>
+      <c r="C360" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D360" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="E360" s="2">
+        <v>0</v>
+      </c>
+      <c r="F360" s="2">
+        <v>7</v>
+      </c>
+      <c r="G360" s="2">
+        <v>0</v>
+      </c>
+      <c r="H360" s="2">
+        <v>0</v>
+      </c>
+      <c r="I360" s="2">
+        <v>7</v>
+      </c>
+      <c r="J360" s="2">
+        <v>52.5</v>
+      </c>
+      <c r="K360" s="2">
+        <v>51.5</v>
+      </c>
+      <c r="L360" s="2">
+        <v>800</v>
+      </c>
+      <c r="M360" s="2">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="361" spans="1:14" x14ac:dyDescent="0.15">
+      <c r="A361" s="2">
+        <v>1023</v>
+      </c>
+      <c r="B361" s="2">
+        <v>388</v>
+      </c>
+      <c r="C361" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D361" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="E361" s="2">
+        <v>7</v>
+      </c>
+      <c r="F361" s="2">
+        <v>21</v>
+      </c>
+      <c r="G361" s="2">
+        <v>0</v>
+      </c>
+      <c r="H361" s="2">
+        <v>17</v>
+      </c>
+      <c r="I361" s="2">
+        <v>45</v>
+      </c>
+      <c r="J361" s="2">
+        <v>16</v>
+      </c>
+      <c r="K361" s="2">
+        <v>20.5</v>
+      </c>
+      <c r="L361" s="2">
+        <v>-1400</v>
+      </c>
+      <c r="M361" s="2">
+        <v>7.5</v>
+      </c>
+    </row>
+    <row r="362" spans="1:14" x14ac:dyDescent="0.15">
+      <c r="A362" s="2">
+        <v>1023</v>
+      </c>
+      <c r="B362" s="2">
+        <v>397</v>
+      </c>
+      <c r="C362" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D362" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="E362" s="2">
+        <v>3</v>
+      </c>
+      <c r="F362" s="2">
+        <v>10</v>
+      </c>
+      <c r="G362" s="2">
+        <v>3</v>
+      </c>
+      <c r="H362" s="2">
+        <v>3</v>
+      </c>
+      <c r="I362" s="2">
+        <v>19</v>
+      </c>
+      <c r="J362" s="2">
+        <v>57</v>
+      </c>
+      <c r="K362" s="2">
+        <v>55.5</v>
+      </c>
+      <c r="L362" s="2">
+        <v>280</v>
+      </c>
+      <c r="M362" s="2">
+        <v>24.5</v>
+      </c>
+    </row>
+    <row r="363" spans="1:14" x14ac:dyDescent="0.15">
+      <c r="A363" s="2">
+        <v>1023</v>
+      </c>
+      <c r="B363" s="2">
+        <v>398</v>
+      </c>
+      <c r="C363" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D363" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="E363" s="2">
+        <v>3</v>
+      </c>
+      <c r="F363" s="2">
+        <v>0</v>
+      </c>
+      <c r="G363" s="2">
+        <v>7</v>
+      </c>
+      <c r="H363" s="2">
+        <v>0</v>
+      </c>
+      <c r="I363" s="2">
+        <v>10</v>
+      </c>
+      <c r="J363" s="2">
+        <v>9.5</v>
+      </c>
+      <c r="K363" s="2">
+        <v>10</v>
+      </c>
+      <c r="L363" s="2">
+        <v>-340</v>
+      </c>
+      <c r="M363" s="2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="364" spans="1:14" x14ac:dyDescent="0.15">
+      <c r="A364" s="2">
+        <v>1024</v>
+      </c>
+      <c r="B364" s="2">
+        <v>311</v>
+      </c>
+      <c r="C364" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D364" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="E364" s="2">
+        <v>0</v>
+      </c>
+      <c r="F364" s="2">
+        <v>14</v>
+      </c>
+      <c r="G364" s="2">
+        <v>7</v>
+      </c>
+      <c r="H364" s="2">
+        <v>6</v>
+      </c>
+      <c r="I364" s="2">
+        <v>27</v>
+      </c>
+      <c r="J364" s="2">
+        <v>56.5</v>
+      </c>
+      <c r="K364" s="2">
+        <v>57</v>
+      </c>
+      <c r="L364" s="2">
+        <v>145</v>
+      </c>
+      <c r="M364" s="2">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="365" spans="1:14" x14ac:dyDescent="0.15">
+      <c r="A365" s="2">
+        <v>1024</v>
+      </c>
+      <c r="B365" s="2">
+        <v>312</v>
+      </c>
+      <c r="C365" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D365" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="E365" s="2">
+        <v>14</v>
+      </c>
+      <c r="F365" s="2">
+        <v>20</v>
+      </c>
+      <c r="G365" s="2">
+        <v>14</v>
+      </c>
+      <c r="H365" s="2">
+        <v>0</v>
+      </c>
+      <c r="I365" s="2">
+        <v>48</v>
+      </c>
+      <c r="J365" s="2">
+        <v>3.5</v>
+      </c>
+      <c r="K365" s="2">
+        <v>3.5</v>
+      </c>
+      <c r="L365" s="2">
+        <v>-165</v>
+      </c>
+      <c r="M365" s="2">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="366" spans="1:14" x14ac:dyDescent="0.15">
+      <c r="A366" s="2">
+        <v>1024</v>
+      </c>
+      <c r="B366" s="2">
+        <v>313</v>
+      </c>
+      <c r="C366" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D366" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="E366" s="2">
+        <v>7</v>
+      </c>
+      <c r="F366" s="2">
+        <v>7</v>
+      </c>
+      <c r="G366" s="2">
+        <v>2</v>
+      </c>
+      <c r="H366" s="2">
+        <v>0</v>
+      </c>
+      <c r="I366" s="2">
+        <v>16</v>
+      </c>
+      <c r="J366" s="2">
+        <v>57</v>
+      </c>
+      <c r="K366" s="2">
+        <v>62</v>
+      </c>
+      <c r="L366" s="2">
+        <v>190</v>
+      </c>
+      <c r="M366" s="2">
+        <v>31.5</v>
+      </c>
+    </row>
+    <row r="367" spans="1:14" x14ac:dyDescent="0.15">
+      <c r="A367" s="2">
+        <v>1024</v>
+      </c>
+      <c r="B367" s="2">
+        <v>314</v>
+      </c>
+      <c r="C367" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D367" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="E367" s="2">
+        <v>21</v>
+      </c>
+      <c r="F367" s="2">
+        <v>10</v>
+      </c>
+      <c r="G367" s="2">
+        <v>7</v>
+      </c>
+      <c r="H367" s="2">
+        <v>10</v>
+      </c>
+      <c r="I367" s="2">
+        <v>48</v>
+      </c>
+      <c r="J367" s="2">
+        <v>6.5</v>
+      </c>
+      <c r="K367" s="2">
+        <v>5.5</v>
+      </c>
+      <c r="L367" s="2">
+        <v>-220</v>
+      </c>
+      <c r="M367" s="2">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="368" spans="1:14" x14ac:dyDescent="0.15">
+      <c r="A368" s="2">
+        <v>1024</v>
+      </c>
+      <c r="B368" s="2">
+        <v>317</v>
+      </c>
+      <c r="C368" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D368" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="E368" s="2">
+        <v>7</v>
+      </c>
+      <c r="F368" s="2">
+        <v>21</v>
+      </c>
+      <c r="G368" s="2">
+        <v>17</v>
+      </c>
+      <c r="H368" s="2">
+        <v>0</v>
+      </c>
+      <c r="I368" s="2">
+        <v>45</v>
+      </c>
+      <c r="J368" s="2">
+        <v>9.5</v>
+      </c>
+      <c r="K368" s="2">
+        <v>10</v>
+      </c>
+      <c r="L368" s="2">
+        <v>-380</v>
+      </c>
+      <c r="M368" s="2">
+        <v>3.5</v>
+      </c>
+    </row>
+    <row r="369" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="A369" s="2">
+        <v>1024</v>
+      </c>
+      <c r="B369" s="2">
+        <v>318</v>
+      </c>
+      <c r="C369" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D369" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="E369" s="2">
+        <v>3</v>
+      </c>
+      <c r="F369" s="2">
+        <v>0</v>
+      </c>
+      <c r="G369" s="2">
+        <v>0</v>
+      </c>
+      <c r="H369" s="2">
+        <v>0</v>
+      </c>
+      <c r="I369" s="2">
+        <v>3</v>
+      </c>
+      <c r="J369" s="2">
+        <v>48</v>
+      </c>
+      <c r="K369" s="2">
+        <v>44</v>
+      </c>
+      <c r="L369" s="2">
+        <v>320</v>
+      </c>
+      <c r="M369" s="2">
+        <v>19.5</v>
+      </c>
+    </row>
+    <row r="370" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="A370" s="2">
+        <v>1024</v>
+      </c>
+      <c r="B370" s="2">
+        <v>319</v>
+      </c>
+      <c r="C370" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D370" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="E370" s="2">
+        <v>14</v>
+      </c>
+      <c r="F370" s="2">
+        <v>14</v>
+      </c>
+      <c r="G370" s="2">
+        <v>14</v>
+      </c>
+      <c r="H370" s="2">
+        <v>6</v>
+      </c>
+      <c r="I370" s="2">
+        <v>48</v>
+      </c>
+      <c r="J370" s="2">
+        <v>18.5</v>
+      </c>
+      <c r="K370" s="2">
+        <v>22</v>
+      </c>
+      <c r="L370" s="2">
+        <v>-2000</v>
+      </c>
+      <c r="M370" s="2">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="371" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="A371" s="2">
+        <v>1024</v>
+      </c>
+      <c r="B371" s="2">
+        <v>320</v>
+      </c>
+      <c r="C371" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D371" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="E371" s="2">
+        <v>0</v>
+      </c>
+      <c r="F371" s="2">
+        <v>10</v>
+      </c>
+      <c r="G371" s="2">
+        <v>7</v>
+      </c>
+      <c r="H371" s="2">
+        <v>0</v>
+      </c>
+      <c r="I371" s="2">
+        <v>17</v>
+      </c>
+      <c r="J371" s="2">
+        <v>62.5</v>
+      </c>
+      <c r="K371" s="2">
+        <v>66.5</v>
+      </c>
+      <c r="L371" s="2">
+        <v>1000</v>
+      </c>
+      <c r="M371" s="2">
+        <v>30.5</v>
+      </c>
+    </row>
+    <row r="372" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="A372" s="2">
+        <v>1024</v>
+      </c>
+      <c r="B372" s="2">
+        <v>321</v>
+      </c>
+      <c r="C372" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D372" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="E372" s="2">
+        <v>0</v>
+      </c>
+      <c r="F372" s="2">
+        <v>7</v>
+      </c>
+      <c r="G372" s="2">
+        <v>7</v>
+      </c>
+      <c r="H372" s="2">
+        <v>7</v>
+      </c>
+      <c r="I372" s="2">
+        <v>21</v>
+      </c>
+      <c r="J372" s="2">
+        <v>64</v>
+      </c>
+      <c r="K372" s="2">
+        <v>61.5</v>
+      </c>
+      <c r="L372" s="2">
+        <v>525</v>
+      </c>
+      <c r="M372" s="2">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="373" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="A373" s="2">
+        <v>1024</v>
+      </c>
+      <c r="B373" s="2">
+        <v>322</v>
+      </c>
+      <c r="C373" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D373" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="E373" s="2">
+        <v>7</v>
+      </c>
+      <c r="F373" s="2">
+        <v>10</v>
+      </c>
+      <c r="G373" s="2">
+        <v>21</v>
+      </c>
+      <c r="H373" s="2">
+        <v>10</v>
+      </c>
+      <c r="I373" s="2">
+        <v>48</v>
+      </c>
+      <c r="J373" s="2">
+        <v>14.5</v>
+      </c>
+      <c r="K373" s="2">
+        <v>15.5</v>
+      </c>
+      <c r="L373" s="2">
+        <v>-750</v>
+      </c>
+      <c r="M373" s="2">
+        <v>7.5</v>
+      </c>
+    </row>
+    <row r="374" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="A374" s="2">
+        <v>1024</v>
+      </c>
+      <c r="B374" s="2">
+        <v>323</v>
+      </c>
+      <c r="C374" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D374" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="E374" s="2">
+        <v>0</v>
+      </c>
+      <c r="F374" s="2">
+        <v>10</v>
+      </c>
+      <c r="G374" s="2">
+        <v>3</v>
+      </c>
+      <c r="H374" s="2">
+        <v>3</v>
+      </c>
+      <c r="I374" s="2">
+        <v>16</v>
+      </c>
+      <c r="J374" s="2">
+        <v>7</v>
+      </c>
+      <c r="K374" s="2">
+        <v>10.5</v>
+      </c>
+      <c r="L374" s="2">
+        <v>-380</v>
+      </c>
+      <c r="M374" s="2">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="375" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="A375" s="2">
+        <v>1024</v>
+      </c>
+      <c r="B375" s="2">
+        <v>324</v>
+      </c>
+      <c r="C375" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D375" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="E375" s="2">
+        <v>10</v>
+      </c>
+      <c r="F375" s="2">
+        <v>7</v>
+      </c>
+      <c r="G375" s="2">
+        <v>3</v>
+      </c>
+      <c r="H375" s="2">
+        <v>3</v>
+      </c>
+      <c r="I375" s="2">
+        <v>23</v>
+      </c>
+      <c r="J375" s="2">
+        <v>70</v>
+      </c>
+      <c r="K375" s="2">
+        <v>68</v>
+      </c>
+      <c r="L375" s="2">
+        <v>320</v>
+      </c>
+      <c r="M375" s="2">
+        <v>32.5</v>
+      </c>
+    </row>
+    <row r="376" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="A376" s="2">
+        <v>1024</v>
+      </c>
+      <c r="B376" s="2">
+        <v>325</v>
+      </c>
+      <c r="C376" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D376" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="E376" s="2">
+        <v>0</v>
+      </c>
+      <c r="F376" s="2">
+        <v>14</v>
+      </c>
+      <c r="G376" s="2">
+        <v>7</v>
+      </c>
+      <c r="H376" s="2">
+        <v>0</v>
+      </c>
+      <c r="I376" s="2">
+        <v>21</v>
+      </c>
+      <c r="J376" s="2">
+        <v>61</v>
+      </c>
+      <c r="K376" s="2">
+        <v>63</v>
+      </c>
+      <c r="L376" s="2">
+        <v>50000</v>
+      </c>
+      <c r="M376" s="2">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="377" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="A377" s="2">
+        <v>1024</v>
+      </c>
+      <c r="B377" s="2">
+        <v>326</v>
+      </c>
+      <c r="C377" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D377" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="E377" s="2">
+        <v>17</v>
+      </c>
+      <c r="F377" s="2">
+        <v>10</v>
+      </c>
+      <c r="G377" s="2">
+        <v>7</v>
+      </c>
+      <c r="H377" s="2">
+        <v>13</v>
+      </c>
+      <c r="I377" s="2">
+        <v>47</v>
+      </c>
+      <c r="J377" s="2">
+        <v>44</v>
+      </c>
+      <c r="K377" s="2">
+        <v>47</v>
+      </c>
+      <c r="L377" s="2">
+        <v>-150000</v>
+      </c>
+      <c r="M377" s="2">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="378" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="A378" s="2">
+        <v>1024</v>
+      </c>
+      <c r="B378" s="2">
+        <v>327</v>
+      </c>
+      <c r="C378" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D378" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="E378" s="2">
+        <v>7</v>
+      </c>
+      <c r="F378" s="2">
+        <v>7</v>
+      </c>
+      <c r="G378" s="2">
+        <v>0</v>
+      </c>
+      <c r="H378" s="2">
+        <v>0</v>
+      </c>
+      <c r="I378" s="2">
+        <v>14</v>
+      </c>
+      <c r="J378" s="2">
+        <v>57</v>
+      </c>
+      <c r="K378" s="2">
+        <v>48.5</v>
+      </c>
+      <c r="L378" s="2">
+        <v>-110</v>
+      </c>
+      <c r="M378" s="2">
+        <v>23.5</v>
+      </c>
+    </row>
+    <row r="379" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="A379" s="2">
+        <v>1024</v>
+      </c>
+      <c r="B379" s="2">
+        <v>328</v>
+      </c>
+      <c r="C379" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D379" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="E379" s="2">
+        <v>7</v>
+      </c>
+      <c r="F379" s="2">
+        <v>7</v>
+      </c>
+      <c r="G379" s="2">
+        <v>0</v>
+      </c>
+      <c r="H379" s="2">
+        <v>14</v>
+      </c>
+      <c r="I379" s="2">
+        <v>28</v>
+      </c>
+      <c r="J379" s="2">
+        <v>4.5</v>
+      </c>
+      <c r="K379" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="L379" s="2">
+        <v>-110</v>
+      </c>
+      <c r="M379" s="2">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="380" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="A380" s="2">
+        <v>1024</v>
+      </c>
+      <c r="B380" s="2">
+        <v>329</v>
+      </c>
+      <c r="C380" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D380" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="E380" s="2">
+        <v>7</v>
+      </c>
+      <c r="F380" s="2">
+        <v>0</v>
+      </c>
+      <c r="G380" s="2">
+        <v>0</v>
+      </c>
+      <c r="H380" s="2">
+        <v>7</v>
+      </c>
+      <c r="I380" s="2">
+        <v>14</v>
+      </c>
+      <c r="J380" s="2">
+        <v>59</v>
+      </c>
+      <c r="K380" s="2">
+        <v>54</v>
+      </c>
+      <c r="L380" s="2">
+        <v>400</v>
+      </c>
+      <c r="M380" s="2">
+        <v>26.5</v>
+      </c>
+    </row>
+    <row r="381" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="A381" s="2">
+        <v>1024</v>
+      </c>
+      <c r="B381" s="2">
+        <v>330</v>
+      </c>
+      <c r="C381" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D381" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="E381" s="2">
+        <v>7</v>
+      </c>
+      <c r="F381" s="2">
+        <v>3</v>
+      </c>
+      <c r="G381" s="2">
+        <v>3</v>
+      </c>
+      <c r="H381" s="2">
+        <v>6</v>
+      </c>
+      <c r="I381" s="2">
+        <v>19</v>
+      </c>
+      <c r="J381" s="2">
+        <v>11</v>
+      </c>
+      <c r="K381" s="2">
+        <v>13.5</v>
+      </c>
+      <c r="L381" s="2">
+        <v>-500</v>
+      </c>
+      <c r="M381" s="2">
+        <v>4.5</v>
+      </c>
+    </row>
+    <row r="382" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="A382" s="2">
+        <v>1024</v>
+      </c>
+      <c r="B382" s="2">
+        <v>331</v>
+      </c>
+      <c r="C382" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D382" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="E382" s="2">
+        <v>14</v>
+      </c>
+      <c r="F382" s="2">
+        <v>0</v>
+      </c>
+      <c r="G382" s="2">
+        <v>14</v>
+      </c>
+      <c r="H382" s="2">
+        <v>6</v>
+      </c>
+      <c r="I382" s="2">
+        <v>34</v>
+      </c>
+      <c r="J382" s="2">
+        <v>73</v>
+      </c>
+      <c r="K382" s="2">
+        <v>71</v>
+      </c>
+      <c r="L382" s="2">
+        <v>850</v>
+      </c>
+      <c r="M382" s="2">
+        <v>31.5</v>
+      </c>
+    </row>
+    <row r="383" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="A383" s="2">
+        <v>1024</v>
+      </c>
+      <c r="B383" s="2">
+        <v>332</v>
+      </c>
+      <c r="C383" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D383" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="E383" s="2">
+        <v>10</v>
+      </c>
+      <c r="F383" s="2">
+        <v>27</v>
+      </c>
+      <c r="G383" s="2">
+        <v>14</v>
+      </c>
+      <c r="H383" s="2">
+        <v>0</v>
+      </c>
+      <c r="I383" s="2">
+        <v>51</v>
+      </c>
+      <c r="J383" s="2">
+        <v>18.5</v>
+      </c>
+      <c r="K383" s="2">
+        <v>21</v>
+      </c>
+      <c r="L383" s="2">
+        <v>-1500</v>
+      </c>
+      <c r="M383" s="2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="384" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="A384" s="2">
+        <v>1024</v>
+      </c>
+      <c r="B384" s="2">
+        <v>335</v>
+      </c>
+      <c r="C384" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D384" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="E384" s="2">
+        <v>3</v>
+      </c>
+      <c r="F384" s="2">
+        <v>13</v>
+      </c>
+      <c r="G384" s="2">
+        <v>7</v>
+      </c>
+      <c r="H384" s="2">
+        <v>14</v>
+      </c>
+      <c r="I384" s="2">
+        <v>37</v>
+      </c>
+      <c r="J384" s="2">
+        <v>12</v>
+      </c>
+      <c r="K384" s="2">
+        <v>15</v>
+      </c>
+      <c r="L384" s="2">
+        <v>-600</v>
+      </c>
+      <c r="M384" s="2">
+        <v>6.5</v>
+      </c>
+    </row>
+    <row r="385" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="A385" s="2">
+        <v>1024</v>
+      </c>
+      <c r="B385" s="2">
+        <v>336</v>
+      </c>
+      <c r="C385" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D385" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="E385" s="2">
+        <v>7</v>
+      </c>
+      <c r="F385" s="2">
+        <v>6</v>
+      </c>
+      <c r="G385" s="2">
+        <v>0</v>
+      </c>
+      <c r="H385" s="2">
+        <v>8</v>
+      </c>
+      <c r="I385" s="2">
+        <v>21</v>
+      </c>
+      <c r="J385" s="2">
+        <v>58</v>
+      </c>
+      <c r="K385" s="2">
+        <v>56.5</v>
+      </c>
+      <c r="L385" s="2">
+        <v>450</v>
+      </c>
+      <c r="M385" s="2">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="386" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="A386" s="2">
+        <v>1024</v>
+      </c>
+      <c r="B386" s="2">
+        <v>337</v>
+      </c>
+      <c r="C386" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D386" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="E386" s="2">
+        <v>7</v>
+      </c>
+      <c r="F386" s="2">
+        <v>0</v>
+      </c>
+      <c r="G386" s="2">
+        <v>7</v>
+      </c>
+      <c r="H386" s="2">
+        <v>14</v>
+      </c>
+      <c r="I386" s="2">
+        <v>35</v>
+      </c>
+      <c r="J386" s="2">
+        <v>7</v>
+      </c>
+      <c r="K386" s="2">
+        <v>6.5</v>
+      </c>
+      <c r="L386" s="2">
+        <v>-260</v>
+      </c>
+      <c r="M386" s="2">
+        <v>4.5</v>
+      </c>
+    </row>
+    <row r="387" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="A387" s="2">
+        <v>1024</v>
+      </c>
+      <c r="B387" s="2">
+        <v>338</v>
+      </c>
+      <c r="C387" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D387" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="E387" s="2">
+        <v>0</v>
+      </c>
+      <c r="F387" s="2">
+        <v>17</v>
+      </c>
+      <c r="G387" s="2">
+        <v>0</v>
+      </c>
+      <c r="H387" s="2">
+        <v>11</v>
+      </c>
+      <c r="I387" s="2">
+        <v>36</v>
+      </c>
+      <c r="J387" s="2">
+        <v>55</v>
+      </c>
+      <c r="K387" s="2">
+        <v>62</v>
+      </c>
+      <c r="L387" s="2">
+        <v>220</v>
+      </c>
+      <c r="M387" s="2">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="388" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="A388" s="2">
+        <v>1024</v>
+      </c>
+      <c r="B388" s="2">
+        <v>339</v>
+      </c>
+      <c r="C388" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D388" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="E388" s="2">
+        <v>14</v>
+      </c>
+      <c r="F388" s="2">
+        <v>14</v>
+      </c>
+      <c r="G388" s="2">
+        <v>0</v>
+      </c>
+      <c r="H388" s="2">
+        <v>10</v>
+      </c>
+      <c r="I388" s="2">
+        <v>38</v>
+      </c>
+      <c r="J388" s="2">
+        <v>47</v>
+      </c>
+      <c r="K388" s="2">
+        <v>44.5</v>
+      </c>
+      <c r="L388" s="2">
+        <v>270</v>
+      </c>
+      <c r="M388" s="2">
+        <v>23.5</v>
+      </c>
+    </row>
+    <row r="389" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="A389" s="2">
+        <v>1024</v>
+      </c>
+      <c r="B389" s="2">
+        <v>340</v>
+      </c>
+      <c r="C389" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D389" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="E389" s="2">
+        <v>7</v>
+      </c>
+      <c r="F389" s="2">
+        <v>6</v>
+      </c>
+      <c r="G389" s="2">
+        <v>7</v>
+      </c>
+      <c r="H389" s="2">
+        <v>7</v>
+      </c>
+      <c r="I389" s="2">
+        <v>27</v>
+      </c>
+      <c r="J389" s="2">
+        <v>16</v>
+      </c>
+      <c r="K389" s="2">
+        <v>9.5</v>
+      </c>
+      <c r="L389" s="2">
+        <v>-330</v>
+      </c>
+      <c r="M389" s="2">
+        <v>7.5</v>
+      </c>
+    </row>
+    <row r="390" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="A390" s="2">
+        <v>1024</v>
+      </c>
+      <c r="B390" s="2">
+        <v>341</v>
+      </c>
+      <c r="C390" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D390" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="E390" s="2">
+        <v>7</v>
+      </c>
+      <c r="F390" s="2">
+        <v>7</v>
+      </c>
+      <c r="G390" s="2">
+        <v>3</v>
+      </c>
+      <c r="H390" s="2">
+        <v>0</v>
+      </c>
+      <c r="I390" s="2">
+        <v>17</v>
+      </c>
+      <c r="J390" s="2">
+        <v>64.5</v>
+      </c>
+      <c r="K390" s="2">
+        <v>69</v>
+      </c>
+      <c r="L390" s="2">
+        <v>1500</v>
+      </c>
+      <c r="M390" s="2">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="391" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="A391" s="2">
+        <v>1024</v>
+      </c>
+      <c r="B391" s="2">
+        <v>342</v>
+      </c>
+      <c r="C391" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D391" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="E391" s="2">
+        <v>14</v>
+      </c>
+      <c r="F391" s="2">
+        <v>10</v>
+      </c>
+      <c r="G391" s="2">
+        <v>14</v>
+      </c>
+      <c r="H391" s="2">
+        <v>14</v>
+      </c>
+      <c r="I391" s="2">
+        <v>52</v>
+      </c>
+      <c r="J391" s="2">
+        <v>25.5</v>
+      </c>
+      <c r="K391" s="2">
+        <v>27.5</v>
+      </c>
+      <c r="L391" s="2">
+        <v>-5000</v>
+      </c>
+      <c r="M391" s="2">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="392" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="A392" s="2">
+        <v>1024</v>
+      </c>
+      <c r="B392" s="2">
+        <v>343</v>
+      </c>
+      <c r="C392" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D392" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="E392" s="2">
+        <v>0</v>
+      </c>
+      <c r="F392" s="2">
+        <v>17</v>
+      </c>
+      <c r="G392" s="2">
+        <v>0</v>
+      </c>
+      <c r="H392" s="2">
+        <v>3</v>
+      </c>
+      <c r="I392" s="2">
+        <v>20</v>
+      </c>
+      <c r="J392" s="2">
+        <v>4</v>
+      </c>
+      <c r="K392" s="2">
+        <v>3</v>
+      </c>
+      <c r="L392" s="2">
+        <v>-150</v>
+      </c>
+      <c r="M392" s="2">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="393" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="A393" s="2">
+        <v>1024</v>
+      </c>
+      <c r="B393" s="2">
+        <v>344</v>
+      </c>
+      <c r="C393" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D393" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="E393" s="2">
+        <v>7</v>
+      </c>
+      <c r="F393" s="2">
+        <v>7</v>
+      </c>
+      <c r="G393" s="2">
+        <v>0</v>
+      </c>
+      <c r="H393" s="2">
+        <v>10</v>
+      </c>
+      <c r="I393" s="2">
+        <v>24</v>
+      </c>
+      <c r="J393" s="2">
+        <v>50.5</v>
+      </c>
+      <c r="K393" s="2">
+        <v>51.5</v>
+      </c>
+      <c r="L393" s="2">
+        <v>130</v>
+      </c>
+      <c r="M393" s="2">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="394" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="A394" s="2">
+        <v>1024</v>
+      </c>
+      <c r="B394" s="2">
+        <v>345</v>
+      </c>
+      <c r="C394" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D394" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="E394" s="2">
+        <v>3</v>
+      </c>
+      <c r="F394" s="2">
+        <v>0</v>
+      </c>
+      <c r="G394" s="2">
+        <v>0</v>
+      </c>
+      <c r="H394" s="2">
+        <v>13</v>
+      </c>
+      <c r="I394" s="2">
+        <v>16</v>
+      </c>
+      <c r="J394" s="2">
+        <v>64</v>
+      </c>
+      <c r="K394" s="2">
+        <v>61.5</v>
+      </c>
+      <c r="L394" s="2">
+        <v>320</v>
+      </c>
+      <c r="M394" s="2">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="395" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="A395" s="2">
+        <v>1024</v>
+      </c>
+      <c r="B395" s="2">
+        <v>346</v>
+      </c>
+      <c r="C395" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D395" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="E395" s="2">
+        <v>0</v>
+      </c>
+      <c r="F395" s="2">
+        <v>13</v>
+      </c>
+      <c r="G395" s="2">
+        <v>14</v>
+      </c>
+      <c r="H395" s="2">
+        <v>0</v>
+      </c>
+      <c r="I395" s="2">
+        <v>27</v>
+      </c>
+      <c r="J395" s="2">
+        <v>10.5</v>
+      </c>
+      <c r="K395" s="2">
+        <v>11</v>
+      </c>
+      <c r="L395" s="2">
+        <v>-380</v>
+      </c>
+      <c r="M395" s="2">
+        <v>4.5</v>
+      </c>
+    </row>
+    <row r="396" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="A396" s="2">
+        <v>1024</v>
+      </c>
+      <c r="B396" s="2">
+        <v>347</v>
+      </c>
+      <c r="C396" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D396" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="E396" s="2">
+        <v>14</v>
+      </c>
+      <c r="F396" s="2">
+        <v>0</v>
+      </c>
+      <c r="G396" s="2">
+        <v>14</v>
+      </c>
+      <c r="H396" s="2">
+        <v>14</v>
+      </c>
+      <c r="I396" s="2">
+        <v>42</v>
+      </c>
+      <c r="J396" s="2">
+        <v>57.5</v>
+      </c>
+      <c r="K396" s="2">
+        <v>57</v>
+      </c>
+      <c r="L396" s="2">
+        <v>-105</v>
+      </c>
+      <c r="M396" s="2">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="397" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="A397" s="2">
+        <v>1024</v>
+      </c>
+      <c r="B397" s="2">
+        <v>348</v>
+      </c>
+      <c r="C397" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D397" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="E397" s="2">
+        <v>0</v>
+      </c>
+      <c r="F397" s="2">
+        <v>10</v>
+      </c>
+      <c r="G397" s="2">
+        <v>0</v>
+      </c>
+      <c r="H397" s="2">
+        <v>3</v>
+      </c>
+      <c r="I397" s="2">
+        <v>13</v>
+      </c>
+      <c r="J397" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="K397" s="2">
+        <v>1</v>
+      </c>
+      <c r="L397" s="2">
+        <v>-115</v>
+      </c>
+      <c r="M397" s="2">
+        <v>27.5</v>
+      </c>
+    </row>
+    <row r="398" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="A398" s="2">
+        <v>1024</v>
+      </c>
+      <c r="B398" s="2">
+        <v>349</v>
+      </c>
+      <c r="C398" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D398" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="E398" s="2">
+        <v>7</v>
+      </c>
+      <c r="F398" s="2">
+        <v>0</v>
+      </c>
+      <c r="G398" s="2">
+        <v>7</v>
+      </c>
+      <c r="H398" s="2">
+        <v>7</v>
+      </c>
+      <c r="I398" s="2">
+        <v>21</v>
+      </c>
+      <c r="J398" s="2">
+        <v>52.5</v>
+      </c>
+      <c r="K398" s="2">
+        <v>54</v>
+      </c>
+      <c r="L398" s="2">
+        <v>115</v>
+      </c>
+      <c r="M398" s="2">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="399" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="A399" s="2">
+        <v>1024</v>
+      </c>
+      <c r="B399" s="2">
+        <v>350</v>
+      </c>
+      <c r="C399" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D399" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="E399" s="2">
+        <v>7</v>
+      </c>
+      <c r="F399" s="2">
+        <v>7</v>
+      </c>
+      <c r="G399" s="2">
+        <v>7</v>
+      </c>
+      <c r="H399" s="2">
+        <v>3</v>
+      </c>
+      <c r="I399" s="2">
+        <v>24</v>
+      </c>
+      <c r="J399" s="2">
+        <v>3.5</v>
+      </c>
+      <c r="K399" s="2">
+        <v>2.5</v>
+      </c>
+      <c r="L399" s="2">
+        <v>-135</v>
+      </c>
+      <c r="M399" s="2">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="400" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="A400" s="2">
+        <v>1024</v>
+      </c>
+      <c r="B400" s="2">
+        <v>351</v>
+      </c>
+      <c r="C400" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D400" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="E400" s="2">
+        <v>10</v>
+      </c>
+      <c r="F400" s="2">
+        <v>7</v>
+      </c>
+      <c r="G400" s="2">
+        <v>10</v>
+      </c>
+      <c r="H400" s="2">
+        <v>6</v>
+      </c>
+      <c r="I400" s="2">
+        <v>33</v>
+      </c>
+      <c r="J400" s="2">
+        <v>6</v>
+      </c>
+      <c r="K400" s="2">
+        <v>6.5</v>
+      </c>
+      <c r="L400" s="2">
+        <v>-250</v>
+      </c>
+      <c r="M400" s="2">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="401" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="A401" s="2">
+        <v>1024</v>
+      </c>
+      <c r="B401" s="2">
+        <v>352</v>
+      </c>
+      <c r="C401" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D401" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="E401" s="2">
+        <v>0</v>
+      </c>
+      <c r="F401" s="2">
+        <v>7</v>
+      </c>
+      <c r="G401" s="2">
+        <v>0</v>
+      </c>
+      <c r="H401" s="2">
+        <v>7</v>
+      </c>
+      <c r="I401" s="2">
+        <v>14</v>
+      </c>
+      <c r="J401" s="2">
+        <v>64</v>
+      </c>
+      <c r="K401" s="2">
+        <v>59</v>
+      </c>
+      <c r="L401" s="2">
+        <v>210</v>
+      </c>
+      <c r="M401" s="2">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="402" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="A402" s="2">
+        <v>1024</v>
+      </c>
+      <c r="B402" s="2">
+        <v>353</v>
+      </c>
+      <c r="C402" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D402" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="E402" s="2">
+        <v>7</v>
+      </c>
+      <c r="F402" s="2">
+        <v>7</v>
+      </c>
+      <c r="G402" s="2">
+        <v>7</v>
+      </c>
+      <c r="H402" s="2">
+        <v>14</v>
+      </c>
+      <c r="I402" s="2">
+        <v>35</v>
+      </c>
+      <c r="J402" s="2">
+        <v>3.5</v>
+      </c>
+      <c r="K402" s="2">
+        <v>3.5</v>
+      </c>
+      <c r="L402" s="2">
+        <v>-170</v>
+      </c>
+      <c r="M402" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="403" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="A403" s="2">
+        <v>1024</v>
+      </c>
+      <c r="B403" s="2">
+        <v>354</v>
+      </c>
+      <c r="C403" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D403" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="E403" s="2">
+        <v>0</v>
+      </c>
+      <c r="F403" s="2">
+        <v>14</v>
+      </c>
+      <c r="G403" s="2">
+        <v>7</v>
+      </c>
+      <c r="H403" s="2">
+        <v>7</v>
+      </c>
+      <c r="I403" s="2">
+        <v>28</v>
+      </c>
+      <c r="J403" s="2">
+        <v>63</v>
+      </c>
+      <c r="K403" s="2">
+        <v>73.5</v>
+      </c>
+      <c r="L403" s="2">
+        <v>150</v>
+      </c>
+      <c r="M403" s="2">
+        <v>36.5</v>
+      </c>
+    </row>
+    <row r="404" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="A404" s="2">
+        <v>1024</v>
+      </c>
+      <c r="B404" s="2">
+        <v>355</v>
+      </c>
+      <c r="C404" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D404" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="E404" s="2">
+        <v>7</v>
+      </c>
+      <c r="F404" s="2">
+        <v>6</v>
+      </c>
+      <c r="G404" s="2">
+        <v>14</v>
+      </c>
+      <c r="H404" s="2">
+        <v>0</v>
+      </c>
+      <c r="I404" s="2">
+        <v>27</v>
+      </c>
+      <c r="J404" s="2">
+        <v>2.5</v>
+      </c>
+      <c r="K404" s="2">
+        <v>2.5</v>
+      </c>
+      <c r="L404" s="2">
+        <v>-140</v>
+      </c>
+      <c r="M404" s="2">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="405" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="A405" s="2">
+        <v>1024</v>
+      </c>
+      <c r="B405" s="2">
+        <v>356</v>
+      </c>
+      <c r="C405" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D405" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="E405" s="2">
+        <v>13</v>
+      </c>
+      <c r="F405" s="2">
+        <v>7</v>
+      </c>
+      <c r="G405" s="2">
+        <v>7</v>
+      </c>
+      <c r="H405" s="2">
+        <v>7</v>
+      </c>
+      <c r="I405" s="2">
+        <v>34</v>
+      </c>
+      <c r="J405" s="2">
+        <v>57</v>
+      </c>
+      <c r="K405" s="2">
+        <v>54</v>
+      </c>
+      <c r="L405" s="2">
+        <v>120</v>
+      </c>
+      <c r="M405" s="2">
+        <v>27.5</v>
+      </c>
+    </row>
+    <row r="406" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="A406" s="2">
+        <v>1024</v>
+      </c>
+      <c r="B406" s="2">
+        <v>357</v>
+      </c>
+      <c r="C406" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D406" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="E406" s="2">
+        <v>3</v>
+      </c>
+      <c r="F406" s="2">
+        <v>12</v>
+      </c>
+      <c r="G406" s="2">
+        <v>7</v>
+      </c>
+      <c r="H406" s="2">
+        <v>7</v>
+      </c>
+      <c r="I406" s="2">
+        <v>29</v>
+      </c>
+      <c r="J406" s="2">
+        <v>69</v>
+      </c>
+      <c r="K406" s="2">
+        <v>70.5</v>
+      </c>
+      <c r="L406" s="2">
+        <v>450</v>
+      </c>
+      <c r="M406" s="2">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="407" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="A407" s="2">
+        <v>1024</v>
+      </c>
+      <c r="B407" s="2">
+        <v>358</v>
+      </c>
+      <c r="C407" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D407" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="E407" s="2">
+        <v>7</v>
+      </c>
+      <c r="F407" s="2">
+        <v>3</v>
+      </c>
+      <c r="G407" s="2">
+        <v>17</v>
+      </c>
+      <c r="H407" s="2">
+        <v>14</v>
+      </c>
+      <c r="I407" s="2">
+        <v>41</v>
+      </c>
+      <c r="J407" s="2">
+        <v>13</v>
+      </c>
+      <c r="K407" s="2">
+        <v>14</v>
+      </c>
+      <c r="L407" s="2">
+        <v>-600</v>
+      </c>
+      <c r="M407" s="2">
+        <v>7.5</v>
+      </c>
+    </row>
+    <row r="408" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="A408" s="2">
+        <v>1024</v>
+      </c>
+      <c r="B408" s="2">
+        <v>359</v>
+      </c>
+      <c r="C408" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D408" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="E408" s="2">
+        <v>0</v>
+      </c>
+      <c r="F408" s="2">
+        <v>7</v>
+      </c>
+      <c r="G408" s="2">
+        <v>0</v>
+      </c>
+      <c r="H408" s="2">
+        <v>7</v>
+      </c>
+      <c r="I408" s="2">
+        <v>14</v>
+      </c>
+      <c r="J408" s="2">
+        <v>54.5</v>
+      </c>
+      <c r="K408" s="2">
+        <v>45.5</v>
+      </c>
+      <c r="L408" s="2">
+        <v>800</v>
+      </c>
+      <c r="M408" s="2">
+        <v>20.5</v>
+      </c>
+    </row>
+    <row r="409" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="A409" s="2">
+        <v>1024</v>
+      </c>
+      <c r="B409" s="2">
+        <v>360</v>
+      </c>
+      <c r="C409" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D409" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="E409" s="2">
+        <v>7</v>
+      </c>
+      <c r="F409" s="2">
+        <v>27</v>
+      </c>
+      <c r="G409" s="2">
+        <v>21</v>
+      </c>
+      <c r="H409" s="2">
+        <v>0</v>
+      </c>
+      <c r="I409" s="2">
+        <v>55</v>
+      </c>
+      <c r="J409" s="2">
+        <v>19</v>
+      </c>
+      <c r="K409" s="2">
+        <v>19.5</v>
+      </c>
+      <c r="L409" s="2">
+        <v>-1400</v>
+      </c>
+      <c r="M409" s="2">
+        <v>7.5</v>
+      </c>
+    </row>
+    <row r="410" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="A410" s="2">
+        <v>1024</v>
+      </c>
+      <c r="B410" s="2">
+        <v>361</v>
+      </c>
+      <c r="C410" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D410" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="E410" s="2">
+        <v>7</v>
+      </c>
+      <c r="F410" s="2">
+        <v>3</v>
+      </c>
+      <c r="G410" s="2">
+        <v>7</v>
+      </c>
+      <c r="H410" s="2">
+        <v>7</v>
+      </c>
+      <c r="I410" s="2">
+        <v>24</v>
+      </c>
+      <c r="J410" s="2">
+        <v>61</v>
+      </c>
+      <c r="K410" s="2">
+        <v>55</v>
+      </c>
+      <c r="L410" s="2">
+        <v>170</v>
+      </c>
+      <c r="M410" s="2">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="411" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="A411" s="2">
+        <v>1024</v>
+      </c>
+      <c r="B411" s="2">
+        <v>362</v>
+      </c>
+      <c r="C411" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D411" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="E411" s="2">
+        <v>10</v>
+      </c>
+      <c r="F411" s="2">
+        <v>21</v>
+      </c>
+      <c r="G411" s="2">
+        <v>14</v>
+      </c>
+      <c r="H411" s="2">
+        <v>7</v>
+      </c>
+      <c r="I411" s="2">
+        <v>52</v>
+      </c>
+      <c r="J411" s="2">
+        <v>6</v>
+      </c>
+      <c r="K411" s="2">
+        <v>4.5</v>
+      </c>
+      <c r="L411" s="2">
+        <v>-190</v>
+      </c>
+      <c r="M411" s="2">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="412" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="A412" s="2">
+        <v>1024</v>
+      </c>
+      <c r="B412" s="2">
+        <v>363</v>
+      </c>
+      <c r="C412" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D412" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="E412" s="2">
+        <v>0</v>
+      </c>
+      <c r="F412" s="2">
+        <v>6</v>
+      </c>
+      <c r="G412" s="2">
+        <v>0</v>
+      </c>
+      <c r="H412" s="2">
+        <v>8</v>
+      </c>
+      <c r="I412" s="2">
+        <v>14</v>
+      </c>
+      <c r="J412" s="2">
+        <v>54</v>
+      </c>
+      <c r="K412" s="2">
+        <v>57</v>
+      </c>
+      <c r="L412" s="2">
+        <v>475</v>
+      </c>
+      <c r="M412" s="2">
+        <v>26.5</v>
+      </c>
+    </row>
+    <row r="413" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="A413" s="2">
+        <v>1024</v>
+      </c>
+      <c r="B413" s="2">
+        <v>364</v>
+      </c>
+      <c r="C413" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D413" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E413" s="2">
+        <v>17</v>
+      </c>
+      <c r="F413" s="2">
+        <v>0</v>
+      </c>
+      <c r="G413" s="2">
+        <v>14</v>
+      </c>
+      <c r="H413" s="2">
+        <v>7</v>
+      </c>
+      <c r="I413" s="2">
+        <v>38</v>
+      </c>
+      <c r="J413" s="2">
+        <v>14</v>
+      </c>
+      <c r="K413" s="2">
+        <v>14.5</v>
+      </c>
+      <c r="L413" s="2">
+        <v>-650</v>
+      </c>
+      <c r="M413" s="2">
+        <v>4.5</v>
+      </c>
+    </row>
+    <row r="414" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="A414" s="2">
+        <v>1024</v>
+      </c>
+      <c r="B414" s="2">
+        <v>365</v>
+      </c>
+      <c r="C414" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D414" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="E414" s="2">
+        <v>3</v>
+      </c>
+      <c r="F414" s="2">
+        <v>0</v>
+      </c>
+      <c r="G414" s="2">
+        <v>0</v>
+      </c>
+      <c r="H414" s="2">
+        <v>0</v>
+      </c>
+      <c r="I414" s="2">
+        <v>3</v>
+      </c>
+      <c r="J414" s="2">
+        <v>51</v>
+      </c>
+      <c r="K414" s="2">
+        <v>53</v>
+      </c>
+      <c r="L414" s="2">
+        <v>400</v>
+      </c>
+      <c r="M414" s="2">
+        <v>21.5</v>
+      </c>
+    </row>
+    <row r="415" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="A415" s="2">
+        <v>1024</v>
+      </c>
+      <c r="B415" s="2">
+        <v>366</v>
+      </c>
+      <c r="C415" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D415" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="E415" s="2">
+        <v>14</v>
+      </c>
+      <c r="F415" s="2">
+        <v>16</v>
+      </c>
+      <c r="G415" s="2">
+        <v>7</v>
+      </c>
+      <c r="H415" s="2">
+        <v>6</v>
+      </c>
+      <c r="I415" s="2">
+        <v>43</v>
+      </c>
+      <c r="J415" s="2">
+        <v>9</v>
+      </c>
+      <c r="K415" s="2">
+        <v>13</v>
+      </c>
+      <c r="L415" s="2">
+        <v>-500</v>
+      </c>
+      <c r="M415" s="2">
+        <v>6.5</v>
+      </c>
+    </row>
+    <row r="416" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="A416" s="2">
+        <v>1024</v>
+      </c>
+      <c r="B416" s="2">
+        <v>367</v>
+      </c>
+      <c r="C416" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D416" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="E416" s="2">
+        <v>7</v>
+      </c>
+      <c r="F416" s="2">
+        <v>0</v>
+      </c>
+      <c r="G416" s="2">
+        <v>0</v>
+      </c>
+      <c r="H416" s="2">
+        <v>7</v>
+      </c>
+      <c r="I416" s="2">
+        <v>14</v>
+      </c>
+      <c r="J416" s="2">
+        <v>58.5</v>
+      </c>
+      <c r="K416" s="2">
+        <v>61.5</v>
+      </c>
+      <c r="L416" s="2">
+        <v>1600</v>
+      </c>
+      <c r="M416" s="2">
+        <v>27.5</v>
+      </c>
+    </row>
+    <row r="417" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="A417" s="2">
+        <v>1024</v>
+      </c>
+      <c r="B417" s="2">
+        <v>368</v>
+      </c>
+      <c r="C417" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D417" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="E417" s="2">
+        <v>14</v>
+      </c>
+      <c r="F417" s="2">
+        <v>21</v>
+      </c>
+      <c r="G417" s="2">
+        <v>14</v>
+      </c>
+      <c r="H417" s="2">
+        <v>3</v>
+      </c>
+      <c r="I417" s="2">
+        <v>52</v>
+      </c>
+      <c r="J417" s="2">
+        <v>30</v>
+      </c>
+      <c r="K417" s="2">
+        <v>29.5</v>
+      </c>
+      <c r="L417" s="2">
+        <v>-6000</v>
+      </c>
+      <c r="M417" s="2">
+        <v>11.5</v>
+      </c>
+    </row>
+    <row r="418" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="A418" s="2">
+        <v>1024</v>
+      </c>
+      <c r="B418" s="2">
+        <v>371</v>
+      </c>
+      <c r="C418" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D418" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="E418" s="2">
+        <v>0</v>
+      </c>
+      <c r="F418" s="2">
+        <v>0</v>
+      </c>
+      <c r="G418" s="2">
+        <v>7</v>
+      </c>
+      <c r="H418" s="2">
+        <v>6</v>
+      </c>
+      <c r="I418" s="2">
+        <v>13</v>
+      </c>
+      <c r="J418" s="2">
+        <v>57.5</v>
+      </c>
+      <c r="K418" s="2">
+        <v>51.5</v>
+      </c>
+      <c r="L418" s="2">
+        <v>600</v>
+      </c>
+      <c r="M418" s="2">
+        <v>20.5</v>
+      </c>
+    </row>
+    <row r="419" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="A419" s="2">
+        <v>1024</v>
+      </c>
+      <c r="B419" s="2">
+        <v>372</v>
+      </c>
+      <c r="C419" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D419" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="E419" s="2">
+        <v>7</v>
+      </c>
+      <c r="F419" s="2">
+        <v>21</v>
+      </c>
+      <c r="G419" s="2">
+        <v>0</v>
+      </c>
+      <c r="H419" s="2">
+        <v>14</v>
+      </c>
+      <c r="I419" s="2">
+        <v>42</v>
+      </c>
+      <c r="J419" s="2">
+        <v>14.5</v>
+      </c>
+      <c r="K419" s="2">
+        <v>17</v>
+      </c>
+      <c r="L419" s="2">
+        <v>-900</v>
+      </c>
+      <c r="M419" s="2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="420" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="A420" s="2">
+        <v>1024</v>
+      </c>
+      <c r="B420" s="2">
+        <v>373</v>
+      </c>
+      <c r="C420" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D420" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="E420" s="2">
+        <v>0</v>
+      </c>
+      <c r="F420" s="2">
+        <v>6</v>
+      </c>
+      <c r="G420" s="2">
+        <v>3</v>
+      </c>
+      <c r="H420" s="2">
+        <v>0</v>
+      </c>
+      <c r="I420" s="2">
+        <v>9</v>
+      </c>
+      <c r="J420" s="2">
+        <v>48.5</v>
+      </c>
+      <c r="K420" s="2">
+        <v>51</v>
+      </c>
+      <c r="L420" s="2">
+        <v>750</v>
+      </c>
+      <c r="M420" s="2">
+        <v>23.5</v>
+      </c>
+    </row>
+    <row r="421" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="A421" s="2">
+        <v>1024</v>
+      </c>
+      <c r="B421" s="2">
+        <v>374</v>
+      </c>
+      <c r="C421" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D421" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="E421" s="2">
+        <v>7</v>
+      </c>
+      <c r="F421" s="2">
+        <v>0</v>
+      </c>
+      <c r="G421" s="2">
+        <v>10</v>
+      </c>
+      <c r="H421" s="2">
+        <v>3</v>
+      </c>
+      <c r="I421" s="2">
+        <v>20</v>
+      </c>
+      <c r="J421" s="2">
+        <v>15</v>
+      </c>
+      <c r="K421" s="2">
+        <v>19.5</v>
+      </c>
+      <c r="L421" s="2">
+        <v>-1200</v>
+      </c>
+      <c r="M421" s="2">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="422" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="A422" s="2">
+        <v>1024</v>
+      </c>
+      <c r="B422" s="2">
+        <v>375</v>
+      </c>
+      <c r="C422" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D422" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="E422" s="2">
+        <v>7</v>
+      </c>
+      <c r="F422" s="2">
+        <v>10</v>
+      </c>
+      <c r="G422" s="2">
+        <v>7</v>
+      </c>
+      <c r="H422" s="2">
+        <v>10</v>
+      </c>
+      <c r="I422" s="2">
+        <v>34</v>
+      </c>
+      <c r="J422" s="2">
+        <v>64.5</v>
+      </c>
+      <c r="K422" s="2">
+        <v>64.5</v>
+      </c>
+      <c r="L422" s="2">
+        <v>130</v>
+      </c>
+      <c r="M422" s="2">
+        <v>30.5</v>
+      </c>
+    </row>
+    <row r="423" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="A423" s="2">
+        <v>1024</v>
+      </c>
+      <c r="B423" s="2">
+        <v>376</v>
+      </c>
+      <c r="C423" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D423" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="E423" s="2">
+        <v>7</v>
+      </c>
+      <c r="F423" s="2">
+        <v>6</v>
+      </c>
+      <c r="G423" s="2">
+        <v>3</v>
+      </c>
+      <c r="H423" s="2">
+        <v>3</v>
+      </c>
+      <c r="I423" s="2">
+        <v>19</v>
+      </c>
+      <c r="J423" s="2">
+        <v>6.5</v>
+      </c>
+      <c r="K423" s="2">
+        <v>3</v>
+      </c>
+      <c r="L423" s="2">
+        <v>-150</v>
+      </c>
+      <c r="M423" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="424" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="A424" s="2">
+        <v>1024</v>
+      </c>
+      <c r="B424" s="2">
+        <v>377</v>
+      </c>
+      <c r="C424" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D424" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="E424" s="2">
+        <v>0</v>
+      </c>
+      <c r="F424" s="2">
+        <v>0</v>
+      </c>
+      <c r="G424" s="2">
+        <v>6</v>
+      </c>
+      <c r="H424" s="2">
+        <v>0</v>
+      </c>
+      <c r="I424" s="2">
+        <v>6</v>
+      </c>
+      <c r="J424" s="2">
+        <v>48</v>
+      </c>
+      <c r="K424" s="2">
+        <v>50.5</v>
+      </c>
+      <c r="L424" s="2">
+        <v>450</v>
+      </c>
+      <c r="M424" s="2">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="425" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="A425" s="2">
+        <v>1024</v>
+      </c>
+      <c r="B425" s="2">
+        <v>378</v>
+      </c>
+      <c r="C425" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D425" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="E425" s="2">
+        <v>7</v>
+      </c>
+      <c r="F425" s="2">
+        <v>20</v>
+      </c>
+      <c r="G425" s="2">
+        <v>0</v>
+      </c>
+      <c r="H425" s="2">
+        <v>7</v>
+      </c>
+      <c r="I425" s="2">
+        <v>34</v>
+      </c>
+      <c r="J425" s="2">
+        <v>14</v>
+      </c>
+      <c r="K425" s="2">
+        <v>14</v>
+      </c>
+      <c r="L425" s="2">
+        <v>-600</v>
+      </c>
+      <c r="M425" s="2">
+        <v>6.5</v>
+      </c>
+    </row>
+    <row r="426" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="A426" s="2">
+        <v>1024</v>
+      </c>
+      <c r="B426" s="2">
+        <v>379</v>
+      </c>
+      <c r="C426" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D426" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="E426" s="2">
+        <v>0</v>
+      </c>
+      <c r="F426" s="2">
+        <v>0</v>
+      </c>
+      <c r="G426" s="2">
+        <v>0</v>
+      </c>
+      <c r="H426" s="2">
+        <v>6</v>
+      </c>
+      <c r="I426" s="2">
+        <v>6</v>
+      </c>
+      <c r="J426" s="2">
+        <v>7</v>
+      </c>
+      <c r="K426" s="2">
+        <v>7.5</v>
+      </c>
+      <c r="L426" s="2">
+        <v>-300</v>
+      </c>
+      <c r="M426" s="2">
+        <v>4.5</v>
+      </c>
+    </row>
+    <row r="427" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="A427" s="2">
+        <v>1024</v>
+      </c>
+      <c r="B427" s="2">
+        <v>380</v>
+      </c>
+      <c r="C427" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D427" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="E427" s="2">
+        <v>0</v>
+      </c>
+      <c r="F427" s="2">
+        <v>0</v>
+      </c>
+      <c r="G427" s="2">
+        <v>14</v>
+      </c>
+      <c r="H427" s="2">
+        <v>3</v>
+      </c>
+      <c r="I427" s="2">
+        <v>17</v>
+      </c>
+      <c r="J427" s="2">
+        <v>60</v>
+      </c>
+      <c r="K427" s="2">
+        <v>64</v>
+      </c>
+      <c r="L427" s="2">
+        <v>250</v>
+      </c>
+      <c r="M427" s="2">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="428" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="A428" s="2">
+        <v>1024</v>
+      </c>
+      <c r="B428" s="2">
+        <v>381</v>
+      </c>
+      <c r="C428" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D428" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="E428" s="2">
+        <v>3</v>
+      </c>
+      <c r="F428" s="2">
+        <v>3</v>
+      </c>
+      <c r="G428" s="2">
+        <v>7</v>
+      </c>
+      <c r="H428" s="2">
+        <v>18</v>
+      </c>
+      <c r="I428" s="2">
+        <v>34</v>
+      </c>
+      <c r="J428" s="2">
+        <v>3</v>
+      </c>
+      <c r="K428" s="2">
+        <v>3</v>
+      </c>
+      <c r="L428" s="2">
+        <v>-150</v>
+      </c>
+      <c r="M428" s="2">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="429" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="A429" s="2">
+        <v>1024</v>
+      </c>
+      <c r="B429" s="2">
+        <v>382</v>
+      </c>
+      <c r="C429" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D429" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="E429" s="2">
+        <v>7</v>
+      </c>
+      <c r="F429" s="2">
+        <v>7</v>
+      </c>
+      <c r="G429" s="2">
+        <v>14</v>
+      </c>
+      <c r="H429" s="2">
+        <v>3</v>
+      </c>
+      <c r="I429" s="2">
+        <v>37</v>
+      </c>
+      <c r="J429" s="2">
+        <v>48</v>
+      </c>
+      <c r="K429" s="2">
+        <v>54</v>
+      </c>
+      <c r="L429" s="2">
+        <v>130</v>
+      </c>
+      <c r="M429" s="2">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="430" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="A430" s="2">
+        <v>1024</v>
+      </c>
+      <c r="B430" s="2">
+        <v>383</v>
+      </c>
+      <c r="C430" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D430" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E430" s="2">
+        <v>7</v>
+      </c>
+      <c r="F430" s="2">
+        <v>0</v>
+      </c>
+      <c r="G430" s="2">
+        <v>21</v>
+      </c>
+      <c r="H430" s="2">
+        <v>7</v>
+      </c>
+      <c r="I430" s="2">
+        <v>35</v>
+      </c>
+      <c r="J430" s="2">
+        <v>63</v>
+      </c>
+      <c r="K430" s="2">
+        <v>60</v>
+      </c>
+      <c r="L430" s="2">
+        <v>500</v>
+      </c>
+      <c r="M430" s="2">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="431" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="A431" s="2">
+        <v>1024</v>
+      </c>
+      <c r="B431" s="2">
+        <v>384</v>
+      </c>
+      <c r="C431" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D431" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="E431" s="2">
+        <v>14</v>
+      </c>
+      <c r="F431" s="2">
+        <v>21</v>
+      </c>
+      <c r="G431" s="2">
+        <v>7</v>
+      </c>
+      <c r="H431" s="2">
+        <v>14</v>
+      </c>
+      <c r="I431" s="2">
+        <v>56</v>
+      </c>
+      <c r="J431" s="2">
+        <v>10.5</v>
+      </c>
+      <c r="K431" s="2">
+        <v>15</v>
+      </c>
+      <c r="L431" s="2">
+        <v>-700</v>
+      </c>
+      <c r="M431" s="2">
+        <v>6.5</v>
+      </c>
+    </row>
+    <row r="432" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="A432" s="2">
+        <v>1024</v>
+      </c>
+      <c r="B432" s="2">
+        <v>385</v>
+      </c>
+      <c r="C432" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D432" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="E432" s="2">
+        <v>21</v>
+      </c>
+      <c r="F432" s="2">
+        <v>14</v>
+      </c>
+      <c r="G432" s="2">
+        <v>7</v>
+      </c>
+      <c r="H432" s="2">
+        <v>7</v>
+      </c>
+      <c r="I432" s="2">
+        <v>49</v>
+      </c>
+      <c r="J432" s="2">
+        <v>3</v>
+      </c>
+      <c r="K432" s="2">
+        <v>3</v>
+      </c>
+      <c r="L432" s="2">
+        <v>-150</v>
+      </c>
+      <c r="M432" s="2">
+        <v>25.5</v>
+      </c>
+    </row>
+    <row r="433" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="A433" s="2">
+        <v>1024</v>
+      </c>
+      <c r="B433" s="2">
+        <v>386</v>
+      </c>
+      <c r="C433" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D433" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="E433" s="2">
+        <v>10</v>
+      </c>
+      <c r="F433" s="2">
+        <v>7</v>
+      </c>
+      <c r="G433" s="2">
+        <v>7</v>
+      </c>
+      <c r="H433" s="2">
+        <v>0</v>
+      </c>
+      <c r="I433" s="2">
+        <v>24</v>
+      </c>
+      <c r="J433" s="2">
+        <v>55</v>
+      </c>
+      <c r="K433" s="2">
+        <v>53.5</v>
+      </c>
+      <c r="L433" s="2">
+        <v>130</v>
+      </c>
+      <c r="M433" s="2">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="434" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="A434" s="2">
+        <v>1024</v>
+      </c>
+      <c r="B434" s="2">
+        <v>389</v>
+      </c>
+      <c r="C434" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D434" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="E434" s="2">
+        <v>7</v>
+      </c>
+      <c r="F434" s="2">
+        <v>6</v>
+      </c>
+      <c r="G434" s="2">
+        <v>20</v>
+      </c>
+      <c r="H434" s="2">
+        <v>3</v>
+      </c>
+      <c r="I434" s="2">
+        <v>36</v>
+      </c>
+      <c r="J434" s="2">
+        <v>70.5</v>
+      </c>
+      <c r="K434" s="2">
+        <v>68.5</v>
+      </c>
+      <c r="L434" s="2">
+        <v>120</v>
+      </c>
+      <c r="M434" s="2">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="435" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="A435" s="2">
+        <v>1024</v>
+      </c>
+      <c r="B435" s="2">
+        <v>390</v>
+      </c>
+      <c r="C435" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D435" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="E435" s="2">
+        <v>7</v>
+      </c>
+      <c r="F435" s="2">
+        <v>14</v>
+      </c>
+      <c r="G435" s="2">
+        <v>0</v>
+      </c>
+      <c r="H435" s="2">
+        <v>13</v>
+      </c>
+      <c r="I435" s="2">
+        <v>34</v>
+      </c>
+      <c r="J435" s="2">
+        <v>1</v>
+      </c>
+      <c r="K435" s="2">
+        <v>2.5</v>
+      </c>
+      <c r="L435" s="2">
+        <v>-140</v>
+      </c>
+      <c r="M435" s="2">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="436" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="A436" s="2">
+        <v>1024</v>
+      </c>
+      <c r="B436" s="2">
+        <v>391</v>
+      </c>
+      <c r="C436" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D436" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="E436" s="2">
+        <v>7</v>
+      </c>
+      <c r="F436" s="2">
+        <v>7</v>
+      </c>
+      <c r="G436" s="2">
+        <v>0</v>
+      </c>
+      <c r="H436" s="2">
+        <v>14</v>
+      </c>
+      <c r="I436" s="2">
+        <v>28</v>
+      </c>
+      <c r="J436" s="2">
+        <v>50.5</v>
+      </c>
+      <c r="K436" s="2">
+        <v>49.5</v>
+      </c>
+      <c r="L436" s="2">
+        <v>650</v>
+      </c>
+      <c r="M436" s="2">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="437" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="A437" s="2">
+        <v>1024</v>
+      </c>
+      <c r="B437" s="2">
+        <v>392</v>
+      </c>
+      <c r="C437" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D437" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="E437" s="2">
+        <v>7</v>
+      </c>
+      <c r="F437" s="2">
+        <v>7</v>
+      </c>
+      <c r="G437" s="2">
+        <v>7</v>
+      </c>
+      <c r="H437" s="2">
+        <v>17</v>
+      </c>
+      <c r="I437" s="2">
+        <v>38</v>
+      </c>
+      <c r="J437" s="2">
+        <v>14</v>
+      </c>
+      <c r="K437" s="2">
+        <v>17.5</v>
+      </c>
+      <c r="L437" s="2">
+        <v>-1000</v>
+      </c>
+      <c r="M437" s="2">
+        <v>7.5</v>
+      </c>
+    </row>
+    <row r="438" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="A438" s="2">
+        <v>1024</v>
+      </c>
+      <c r="B438" s="2">
+        <v>393</v>
+      </c>
+      <c r="C438" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D438" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="E438" s="2">
+        <v>0</v>
+      </c>
+      <c r="F438" s="2">
+        <v>14</v>
+      </c>
+      <c r="G438" s="2">
+        <v>17</v>
+      </c>
+      <c r="H438" s="2">
+        <v>3</v>
+      </c>
+      <c r="I438" s="2">
+        <v>40</v>
+      </c>
+      <c r="J438" s="2">
+        <v>51</v>
+      </c>
+      <c r="K438" s="2">
+        <v>49</v>
+      </c>
+      <c r="L438" s="2">
+        <v>165</v>
+      </c>
+      <c r="M438" s="2">
+        <v>24.5</v>
+      </c>
+    </row>
+    <row r="439" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="A439" s="2">
+        <v>1024</v>
+      </c>
+      <c r="B439" s="2">
+        <v>394</v>
+      </c>
+      <c r="C439" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D439" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="E439" s="2">
+        <v>6</v>
+      </c>
+      <c r="F439" s="2">
+        <v>7</v>
+      </c>
+      <c r="G439" s="2">
+        <v>6</v>
+      </c>
+      <c r="H439" s="2">
+        <v>15</v>
+      </c>
+      <c r="I439" s="2">
+        <v>34</v>
+      </c>
+      <c r="J439" s="2">
+        <v>1</v>
+      </c>
+      <c r="K439" s="2">
+        <v>4.5</v>
+      </c>
+      <c r="L439" s="2">
+        <v>-185</v>
+      </c>
+      <c r="M439" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="440" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="A440" s="2">
+        <v>1024</v>
+      </c>
+      <c r="B440" s="2">
+        <v>395</v>
+      </c>
+      <c r="C440" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D440" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="E440" s="2">
+        <v>3</v>
+      </c>
+      <c r="F440" s="2">
+        <v>16</v>
+      </c>
+      <c r="G440" s="2">
+        <v>7</v>
+      </c>
+      <c r="H440" s="2">
+        <v>0</v>
+      </c>
+      <c r="I440" s="2">
+        <v>26</v>
+      </c>
+      <c r="J440" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="K440" s="2">
+        <v>2.5</v>
+      </c>
+      <c r="L440" s="2">
+        <v>-140</v>
+      </c>
+      <c r="M440" s="2">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="441" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="A441" s="2">
+        <v>1024</v>
+      </c>
+      <c r="B441" s="2">
+        <v>396</v>
+      </c>
+      <c r="C441" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D441" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="E441" s="2">
+        <v>3</v>
+      </c>
+      <c r="F441" s="2">
+        <v>3</v>
+      </c>
+      <c r="G441" s="2">
+        <v>7</v>
+      </c>
+      <c r="H441" s="2">
+        <v>14</v>
+      </c>
+      <c r="I441" s="2">
+        <v>27</v>
+      </c>
+      <c r="J441" s="2">
+        <v>55</v>
+      </c>
+      <c r="K441" s="2">
+        <v>54</v>
+      </c>
+      <c r="L441" s="2">
+        <v>120</v>
+      </c>
+      <c r="M441" s="2">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="442" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="A442" s="2">
+        <v>1024</v>
+      </c>
+      <c r="B442" s="2">
+        <v>399</v>
+      </c>
+      <c r="C442" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D442" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="E442" s="2">
+        <v>3</v>
+      </c>
+      <c r="F442" s="2">
+        <v>0</v>
+      </c>
+      <c r="G442" s="2">
+        <v>0</v>
+      </c>
+      <c r="H442" s="2">
+        <v>0</v>
+      </c>
+      <c r="I442" s="2">
+        <v>3</v>
+      </c>
+      <c r="J442" s="2">
+        <v>50</v>
+      </c>
+      <c r="K442" s="2">
+        <v>47.5</v>
+      </c>
+      <c r="L442" s="2">
+        <v>2000</v>
+      </c>
+      <c r="M442" s="2">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="443" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="A443" s="2">
+        <v>1024</v>
+      </c>
+      <c r="B443" s="2">
+        <v>400</v>
+      </c>
+      <c r="C443" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D443" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="E443" s="2">
+        <v>7</v>
+      </c>
+      <c r="F443" s="2">
+        <v>14</v>
+      </c>
+      <c r="G443" s="2">
+        <v>21</v>
+      </c>
+      <c r="H443" s="2">
+        <v>7</v>
+      </c>
+      <c r="I443" s="2">
+        <v>49</v>
+      </c>
+      <c r="J443" s="2">
+        <v>30</v>
+      </c>
+      <c r="K443" s="2">
+        <v>30</v>
+      </c>
+      <c r="L443" s="2">
+        <v>-10000</v>
+      </c>
+      <c r="M443" s="2">
+        <v>21.5</v>
+      </c>
+    </row>
+    <row r="444" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="A444" s="2">
+        <v>1024</v>
+      </c>
+      <c r="B444" s="2">
+        <v>401</v>
+      </c>
+      <c r="C444" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D444" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="E444" s="2">
+        <v>7</v>
+      </c>
+      <c r="F444" s="2">
+        <v>0</v>
+      </c>
+      <c r="G444" s="2">
+        <v>3</v>
+      </c>
+      <c r="H444" s="2">
+        <v>0</v>
+      </c>
+      <c r="I444" s="2">
+        <v>10</v>
+      </c>
+      <c r="J444" s="2">
+        <v>55</v>
+      </c>
+      <c r="K444" s="2">
+        <v>53.5</v>
+      </c>
+      <c r="L444" s="2">
+        <v>475</v>
+      </c>
+      <c r="M444" s="2">
+        <v>19.5</v>
+      </c>
+    </row>
+    <row r="445" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="A445" s="2">
+        <v>1024</v>
+      </c>
+      <c r="B445" s="2">
+        <v>402</v>
+      </c>
+      <c r="C445" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D445" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="E445" s="2">
+        <v>3</v>
+      </c>
+      <c r="F445" s="2">
+        <v>0</v>
+      </c>
+      <c r="G445" s="2">
+        <v>3</v>
+      </c>
+      <c r="H445" s="2">
+        <v>7</v>
+      </c>
+      <c r="I445" s="2">
+        <v>13</v>
+      </c>
+      <c r="J445" s="2">
+        <v>13</v>
+      </c>
+      <c r="K445" s="2">
+        <v>14.5</v>
+      </c>
+      <c r="L445" s="2">
+        <v>-650</v>
+      </c>
+      <c r="M445" s="2">
+        <v>10.5</v>
+      </c>
+    </row>
+    <row r="446" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="A446" s="2">
+        <v>1024</v>
+      </c>
+      <c r="B446" s="2">
+        <v>403</v>
+      </c>
+      <c r="C446" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D446" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="E446" s="2">
+        <v>0</v>
+      </c>
+      <c r="F446" s="2">
+        <v>3</v>
+      </c>
+      <c r="G446" s="2">
+        <v>0</v>
+      </c>
+      <c r="H446" s="2">
+        <v>7</v>
+      </c>
+      <c r="I446" s="2">
+        <v>10</v>
+      </c>
+      <c r="J446" s="2">
+        <v>6</v>
+      </c>
+      <c r="K446" s="2">
+        <v>3</v>
+      </c>
+      <c r="L446" s="2">
+        <v>-150</v>
+      </c>
+      <c r="M446" s="2">
+        <v>24.5</v>
+      </c>
+    </row>
+    <row r="447" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="A447" s="2">
+        <v>1024</v>
+      </c>
+      <c r="B447" s="2">
+        <v>404</v>
+      </c>
+      <c r="C447" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D447" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="E447" s="2">
+        <v>0</v>
+      </c>
+      <c r="F447" s="2">
+        <v>10</v>
+      </c>
+      <c r="G447" s="2">
+        <v>7</v>
+      </c>
+      <c r="H447" s="2">
+        <v>3</v>
+      </c>
+      <c r="I447" s="2">
+        <v>20</v>
+      </c>
+      <c r="J447" s="2">
+        <v>50.5</v>
+      </c>
+      <c r="K447" s="2">
+        <v>47</v>
+      </c>
+      <c r="L447" s="2">
+        <v>130</v>
+      </c>
+      <c r="M447" s="2">
+        <v>7.5</v>
+      </c>
+    </row>
+    <row r="448" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="A448" s="2">
+        <v>1024</v>
+      </c>
+      <c r="B448" s="2">
+        <v>308901</v>
+      </c>
+      <c r="C448" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D448" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="E448" s="2">
+        <v>0</v>
+      </c>
+      <c r="F448" s="2">
+        <v>7</v>
+      </c>
+      <c r="G448" s="2">
+        <v>6</v>
+      </c>
+      <c r="H448" s="2">
+        <v>16</v>
+      </c>
+      <c r="I448" s="2">
+        <v>35</v>
+      </c>
+      <c r="J448" s="2">
+        <v>48.5</v>
+      </c>
+      <c r="K448" s="2">
+        <v>50.5</v>
+      </c>
+      <c r="L448" s="2">
+        <v>130</v>
+      </c>
+      <c r="M448" s="2">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="449" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="A449" s="2">
+        <v>1024</v>
+      </c>
+      <c r="B449" s="2">
+        <v>308902</v>
+      </c>
+      <c r="C449" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D449" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="E449" s="2">
+        <v>7</v>
+      </c>
+      <c r="F449" s="2">
+        <v>7</v>
+      </c>
+      <c r="G449" s="2">
+        <v>0</v>
+      </c>
+      <c r="H449" s="2">
+        <v>15</v>
+      </c>
+      <c r="I449" s="2">
+        <v>32</v>
+      </c>
+      <c r="J449" s="2">
+        <v>2.5</v>
+      </c>
+      <c r="K449" s="2">
+        <v>3</v>
+      </c>
+      <c r="L449" s="2">
+        <v>-150</v>
+      </c>
+      <c r="M449" s="2">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="450" spans="1:13" ht="9" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="451" spans="1:13" ht="9" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="452" spans="1:13" ht="9" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="453" spans="1:13" ht="9" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="454" spans="1:13" ht="9" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="455" spans="1:13" ht="9" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="456" spans="1:13" ht="9" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="457" spans="1:13" ht="9" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="458" spans="1:13" ht="9" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="459" spans="1:13" ht="9" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="460" spans="1:13" ht="9" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="461" spans="1:13" ht="9" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="462" spans="1:13" ht="9" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="463" spans="1:13" ht="9" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="464" spans="1:13" ht="9" customHeight="1" x14ac:dyDescent="0.15"/>
     <row r="465" ht="9" customHeight="1" x14ac:dyDescent="0.15"/>
     <row r="466" ht="9" customHeight="1" x14ac:dyDescent="0.15"/>
     <row r="467" ht="9" customHeight="1" x14ac:dyDescent="0.15"/>

</xml_diff>